<commit_message>
Adaugare campanii de catre admin in pagina
</commit_message>
<xml_diff>
--- a/src/api/utils/statistici/confiscari-2021.xlsx
+++ b/src/api/utils/statistici/confiscari-2021.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Facultate\Proiect-Tw\src\api\utils\statistici\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ycarp\Desktop\cloneMihaiA2-a\Proiect-Tw\src\api\utils\statistici\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B094B9FB-18E4-45CB-BA68-94DA37E577FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="0"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Heroină</t>
   </si>
@@ -130,28 +130,19 @@
   </si>
   <si>
     <t>Capturi</t>
-  </si>
-  <si>
-    <t>103,24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -198,121 +189,31 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -586,20 +487,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" activeCellId="1" sqref="E22 G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.714285714285715" customWidth="1"/>
-    <col min="2" max="6" width="11.714285714285714" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -619,7 +520,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -633,7 +534,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -647,7 +548,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -659,13 +560,13 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1">
-        <v>1.90</v>
+        <v>1.9</v>
       </c>
       <c r="F4" s="1">
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -681,7 +582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -697,7 +598,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -715,7 +616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -731,25 +632,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>38.02</v>
+        <v>38.020000000000003</v>
       </c>
       <c r="C9" s="1">
         <v>52</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1">
-        <v>43.70</v>
+        <v>43.7</v>
       </c>
       <c r="F9" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -761,13 +662,13 @@
         <v>1541</v>
       </c>
       <c r="E10" s="1">
-        <v>4.70</v>
+        <v>4.7</v>
       </c>
       <c r="F10" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -783,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -797,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -811,7 +712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -825,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -841,7 +742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -857,7 +758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -873,7 +774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -889,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -903,7 +804,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -917,7 +818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -925,13 +826,13 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1">
-        <v>11.40</v>
+        <v>11.4</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -940,14 +841,14 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>35</v>
+      <c r="E22" s="5">
+        <v>103.24</v>
       </c>
       <c r="F22" s="1">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -965,12 +866,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>0.90</v>
+        <v>0.9</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -979,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
@@ -993,7 +894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -1021,12 +922,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="1">
-        <v>1.70</v>
+        <v>1.7</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1035,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
@@ -1051,7 +952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
@@ -1065,7 +966,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
@@ -1081,6 +982,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="90" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>